<commit_message>
changed battery charging logic, added back excess energy vwap and new chart logic
</commit_message>
<xml_diff>
--- a/data/Simulator output.xlsx
+++ b/data/Simulator output.xlsx
@@ -506,7 +506,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AY24"/>
+  <dimension ref="A1:BE34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" zoomScale="81" workbookViewId="0">
       <selection activeCell="G184" sqref="G184"/>
@@ -1952,7 +1952,6 @@
       <c r="AF20" t="n">
         <v>0</v>
       </c>
-      <c r="AG20" t="inlineStr"/>
       <c r="AH20" t="n">
         <v>44</v>
       </c>
@@ -2102,7 +2101,6 @@
       <c r="AF21" t="n">
         <v>0</v>
       </c>
-      <c r="AG21" t="inlineStr"/>
       <c r="AH21" t="n">
         <v>44</v>
       </c>
@@ -2252,7 +2250,6 @@
       <c r="AF22" t="n">
         <v>0</v>
       </c>
-      <c r="AG22" t="inlineStr"/>
       <c r="AH22" t="n">
         <v>44</v>
       </c>
@@ -2402,7 +2399,6 @@
       <c r="AF23" t="n">
         <v>0</v>
       </c>
-      <c r="AG23" t="inlineStr"/>
       <c r="AH23" t="n">
         <v>44</v>
       </c>
@@ -2552,7 +2548,6 @@
       <c r="AF24" t="n">
         <v>0</v>
       </c>
-      <c r="AG24" t="inlineStr"/>
       <c r="AH24" t="n">
         <v>44</v>
       </c>
@@ -2606,6 +2601,1706 @@
       </c>
       <c r="AY24" t="n">
         <v>60</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>2020</v>
+      </c>
+      <c r="D25" t="n">
+        <v>78.86</v>
+      </c>
+      <c r="E25" t="n">
+        <v>78.86</v>
+      </c>
+      <c r="F25" t="n">
+        <v>135.71</v>
+      </c>
+      <c r="G25" t="n">
+        <v>135.71</v>
+      </c>
+      <c r="H25" t="n">
+        <v>69.69</v>
+      </c>
+      <c r="I25" t="n">
+        <v>33.69231955828779</v>
+      </c>
+      <c r="J25" t="n">
+        <v>100</v>
+      </c>
+      <c r="K25" t="n">
+        <v>8784</v>
+      </c>
+      <c r="L25" t="n">
+        <v>8784</v>
+      </c>
+      <c r="M25" t="n">
+        <v>30.56</v>
+      </c>
+      <c r="N25" t="n">
+        <v>41</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>36.12</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>87840</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="n">
+        <v>1368.1</v>
+      </c>
+      <c r="T25" t="n">
+        <v>158400</v>
+      </c>
+      <c r="U25" t="n">
+        <v>137483</v>
+      </c>
+      <c r="V25" t="n">
+        <v>47803</v>
+      </c>
+      <c r="W25" t="n">
+        <v>22287</v>
+      </c>
+      <c r="X25" t="n">
+        <v>96394</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>109819</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN25" t="n">
+        <v>44</v>
+      </c>
+      <c r="AO25" t="n">
+        <v>183</v>
+      </c>
+      <c r="AP25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR25" t="n">
+        <v>150</v>
+      </c>
+      <c r="AS25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV25" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW25" t="n">
+        <v>50</v>
+      </c>
+      <c r="AX25" t="n">
+        <v>60</v>
+      </c>
+      <c r="AY25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA25" t="n">
+        <v>3200000</v>
+      </c>
+      <c r="BB25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE25" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D26" t="n">
+        <v>77.59999999999999</v>
+      </c>
+      <c r="E26" t="n">
+        <v>77.59999999999999</v>
+      </c>
+      <c r="F26" t="n">
+        <v>28.98</v>
+      </c>
+      <c r="G26" t="n">
+        <v>28.98</v>
+      </c>
+      <c r="H26" t="n">
+        <v>68.98</v>
+      </c>
+      <c r="I26" t="n">
+        <v>86.7317895878525</v>
+      </c>
+      <c r="J26" t="n">
+        <v>100</v>
+      </c>
+      <c r="K26" t="n">
+        <v>8758</v>
+      </c>
+      <c r="L26" t="n">
+        <v>8759</v>
+      </c>
+      <c r="M26" t="n">
+        <v>85.67</v>
+      </c>
+      <c r="N26" t="n">
+        <v>83.28</v>
+      </c>
+      <c r="O26" t="n">
+        <v>10.31</v>
+      </c>
+      <c r="P26" t="n">
+        <v>83.52</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>87590</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" t="n">
+        <v>1498.68</v>
+      </c>
+      <c r="T26" t="n">
+        <v>134772</v>
+      </c>
+      <c r="U26" t="n">
+        <v>152631</v>
+      </c>
+      <c r="V26" t="n">
+        <v>44173</v>
+      </c>
+      <c r="W26" t="n">
+        <v>23137</v>
+      </c>
+      <c r="X26" t="n">
+        <v>74723</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>123526</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN26" t="n">
+        <v>44</v>
+      </c>
+      <c r="AO26" t="n">
+        <v>183</v>
+      </c>
+      <c r="AP26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR26" t="n">
+        <v>150</v>
+      </c>
+      <c r="AS26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV26" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW26" t="n">
+        <v>50</v>
+      </c>
+      <c r="AX26" t="n">
+        <v>60</v>
+      </c>
+      <c r="AY26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA26" t="n">
+        <v>3200000</v>
+      </c>
+      <c r="BB26" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC26" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD26" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE26" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D27" t="n">
+        <v>73.56</v>
+      </c>
+      <c r="E27" t="n">
+        <v>73.56</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-227.96</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-227.96</v>
+      </c>
+      <c r="H27" t="n">
+        <v>70.7</v>
+      </c>
+      <c r="I27" t="n">
+        <v>192.8286214179701</v>
+      </c>
+      <c r="J27" t="n">
+        <v>99.01000000000001</v>
+      </c>
+      <c r="K27" t="n">
+        <v>8576</v>
+      </c>
+      <c r="L27" t="n">
+        <v>8759</v>
+      </c>
+      <c r="M27" t="n">
+        <v>159.18</v>
+      </c>
+      <c r="N27" t="n">
+        <v>203.63</v>
+      </c>
+      <c r="O27" t="n">
+        <v>328.35</v>
+      </c>
+      <c r="P27" t="n">
+        <v>187.95</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>87590</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" t="n">
+        <v>2040.93</v>
+      </c>
+      <c r="T27" t="n">
+        <v>106480</v>
+      </c>
+      <c r="U27" t="n">
+        <v>196762</v>
+      </c>
+      <c r="V27" t="n">
+        <v>33035</v>
+      </c>
+      <c r="W27" t="n">
+        <v>26525</v>
+      </c>
+      <c r="X27" t="n">
+        <v>52518</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>161883</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN27" t="n">
+        <v>44</v>
+      </c>
+      <c r="AO27" t="n">
+        <v>183</v>
+      </c>
+      <c r="AP27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR27" t="n">
+        <v>150</v>
+      </c>
+      <c r="AS27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV27" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW27" t="n">
+        <v>50</v>
+      </c>
+      <c r="AX27" t="n">
+        <v>60</v>
+      </c>
+      <c r="AY27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA27" t="n">
+        <v>3200000</v>
+      </c>
+      <c r="BB27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE27" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D28" t="n">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="E28" t="n">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="F28" t="n">
+        <v>53.11</v>
+      </c>
+      <c r="G28" t="n">
+        <v>53.11</v>
+      </c>
+      <c r="H28" t="n">
+        <v>72.56</v>
+      </c>
+      <c r="I28" t="n">
+        <v>90.80076435666172</v>
+      </c>
+      <c r="J28" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="K28" t="n">
+        <v>8719</v>
+      </c>
+      <c r="L28" t="n">
+        <v>8759</v>
+      </c>
+      <c r="M28" t="n">
+        <v>78.72</v>
+      </c>
+      <c r="N28" t="n">
+        <v>73.3</v>
+      </c>
+      <c r="O28" t="n">
+        <v>173.88</v>
+      </c>
+      <c r="P28" t="n">
+        <v>71.29000000000001</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>87590</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" t="n">
+        <v>1754.68</v>
+      </c>
+      <c r="T28" t="n">
+        <v>123200</v>
+      </c>
+      <c r="U28" t="n">
+        <v>201300</v>
+      </c>
+      <c r="V28" t="n">
+        <v>36744</v>
+      </c>
+      <c r="W28" t="n">
+        <v>27146</v>
+      </c>
+      <c r="X28" t="n">
+        <v>67653</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>167810</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN28" t="n">
+        <v>44</v>
+      </c>
+      <c r="AO28" t="n">
+        <v>183</v>
+      </c>
+      <c r="AP28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR28" t="n">
+        <v>150</v>
+      </c>
+      <c r="AS28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV28" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW28" t="n">
+        <v>50</v>
+      </c>
+      <c r="AX28" t="n">
+        <v>60</v>
+      </c>
+      <c r="AY28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ28" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA28" t="n">
+        <v>3200000</v>
+      </c>
+      <c r="BB28" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC28" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD28" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE28" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" t="n">
+        <v>2024</v>
+      </c>
+      <c r="D29" t="n">
+        <v>79.11</v>
+      </c>
+      <c r="E29" t="n">
+        <v>79.11</v>
+      </c>
+      <c r="F29" t="n">
+        <v>71.54000000000001</v>
+      </c>
+      <c r="G29" t="n">
+        <v>71.54000000000001</v>
+      </c>
+      <c r="H29" t="n">
+        <v>75.48</v>
+      </c>
+      <c r="I29" t="n">
+        <v>87.26646435891597</v>
+      </c>
+      <c r="J29" t="n">
+        <v>100</v>
+      </c>
+      <c r="K29" t="n">
+        <v>8782</v>
+      </c>
+      <c r="L29" t="n">
+        <v>8782</v>
+      </c>
+      <c r="M29" t="n">
+        <v>72.68000000000001</v>
+      </c>
+      <c r="N29" t="n">
+        <v>64.28</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="n">
+        <v>63.02</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>87820</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" t="n">
+        <v>1571.08</v>
+      </c>
+      <c r="T29" t="n">
+        <v>145200</v>
+      </c>
+      <c r="U29" t="n">
+        <v>219600</v>
+      </c>
+      <c r="V29" t="n">
+        <v>41442</v>
+      </c>
+      <c r="W29" t="n">
+        <v>27918</v>
+      </c>
+      <c r="X29" t="n">
+        <v>91709</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>183657</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN29" t="n">
+        <v>44</v>
+      </c>
+      <c r="AO29" t="n">
+        <v>183</v>
+      </c>
+      <c r="AP29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR29" t="n">
+        <v>150</v>
+      </c>
+      <c r="AS29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV29" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW29" t="n">
+        <v>50</v>
+      </c>
+      <c r="AX29" t="n">
+        <v>60</v>
+      </c>
+      <c r="AY29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ29" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA29" t="n">
+        <v>3200000</v>
+      </c>
+      <c r="BB29" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC29" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD29" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE29" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" t="n">
+        <v>2020</v>
+      </c>
+      <c r="D30" t="n">
+        <v>78.86</v>
+      </c>
+      <c r="E30" t="n">
+        <v>78.86</v>
+      </c>
+      <c r="F30" t="n">
+        <v>135.71</v>
+      </c>
+      <c r="G30" t="n">
+        <v>135.71</v>
+      </c>
+      <c r="H30" t="n">
+        <v>69.69</v>
+      </c>
+      <c r="I30" t="n">
+        <v>33.69231955828779</v>
+      </c>
+      <c r="J30" t="n">
+        <v>100</v>
+      </c>
+      <c r="K30" t="n">
+        <v>8784</v>
+      </c>
+      <c r="L30" t="n">
+        <v>8784</v>
+      </c>
+      <c r="M30" t="n">
+        <v>30.56</v>
+      </c>
+      <c r="N30" t="n">
+        <v>41</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>36.12</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>87840</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="n">
+        <v>1368.1</v>
+      </c>
+      <c r="T30" t="n">
+        <v>158400</v>
+      </c>
+      <c r="U30" t="n">
+        <v>137483</v>
+      </c>
+      <c r="V30" t="n">
+        <v>47803</v>
+      </c>
+      <c r="W30" t="n">
+        <v>22287</v>
+      </c>
+      <c r="X30" t="n">
+        <v>96394</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>109819</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN30" t="n">
+        <v>44</v>
+      </c>
+      <c r="AO30" t="n">
+        <v>183</v>
+      </c>
+      <c r="AP30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR30" t="n">
+        <v>150</v>
+      </c>
+      <c r="AS30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV30" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW30" t="n">
+        <v>50</v>
+      </c>
+      <c r="AX30" t="n">
+        <v>60</v>
+      </c>
+      <c r="AY30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA30" t="n">
+        <v>3200000</v>
+      </c>
+      <c r="BB30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE30" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D31" t="n">
+        <v>77.59999999999999</v>
+      </c>
+      <c r="E31" t="n">
+        <v>77.59999999999999</v>
+      </c>
+      <c r="F31" t="n">
+        <v>28.98</v>
+      </c>
+      <c r="G31" t="n">
+        <v>28.98</v>
+      </c>
+      <c r="H31" t="n">
+        <v>68.98</v>
+      </c>
+      <c r="I31" t="n">
+        <v>86.7317895878525</v>
+      </c>
+      <c r="J31" t="n">
+        <v>100</v>
+      </c>
+      <c r="K31" t="n">
+        <v>8758</v>
+      </c>
+      <c r="L31" t="n">
+        <v>8759</v>
+      </c>
+      <c r="M31" t="n">
+        <v>85.67</v>
+      </c>
+      <c r="N31" t="n">
+        <v>83.28</v>
+      </c>
+      <c r="O31" t="n">
+        <v>10.31</v>
+      </c>
+      <c r="P31" t="n">
+        <v>83.52</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>87590</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" t="n">
+        <v>1498.68</v>
+      </c>
+      <c r="T31" t="n">
+        <v>134772</v>
+      </c>
+      <c r="U31" t="n">
+        <v>152631</v>
+      </c>
+      <c r="V31" t="n">
+        <v>44173</v>
+      </c>
+      <c r="W31" t="n">
+        <v>23137</v>
+      </c>
+      <c r="X31" t="n">
+        <v>74723</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>123526</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN31" t="n">
+        <v>44</v>
+      </c>
+      <c r="AO31" t="n">
+        <v>183</v>
+      </c>
+      <c r="AP31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR31" t="n">
+        <v>150</v>
+      </c>
+      <c r="AS31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV31" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW31" t="n">
+        <v>50</v>
+      </c>
+      <c r="AX31" t="n">
+        <v>60</v>
+      </c>
+      <c r="AY31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA31" t="n">
+        <v>3200000</v>
+      </c>
+      <c r="BB31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE31" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D32" t="n">
+        <v>73.56</v>
+      </c>
+      <c r="E32" t="n">
+        <v>73.56</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-227.96</v>
+      </c>
+      <c r="G32" t="n">
+        <v>-227.96</v>
+      </c>
+      <c r="H32" t="n">
+        <v>70.7</v>
+      </c>
+      <c r="I32" t="n">
+        <v>192.8286214179701</v>
+      </c>
+      <c r="J32" t="n">
+        <v>99.01000000000001</v>
+      </c>
+      <c r="K32" t="n">
+        <v>8576</v>
+      </c>
+      <c r="L32" t="n">
+        <v>8759</v>
+      </c>
+      <c r="M32" t="n">
+        <v>159.18</v>
+      </c>
+      <c r="N32" t="n">
+        <v>203.63</v>
+      </c>
+      <c r="O32" t="n">
+        <v>328.35</v>
+      </c>
+      <c r="P32" t="n">
+        <v>187.95</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>87590</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>2040.93</v>
+      </c>
+      <c r="T32" t="n">
+        <v>106480</v>
+      </c>
+      <c r="U32" t="n">
+        <v>196762</v>
+      </c>
+      <c r="V32" t="n">
+        <v>33035</v>
+      </c>
+      <c r="W32" t="n">
+        <v>26525</v>
+      </c>
+      <c r="X32" t="n">
+        <v>52518</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>161883</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN32" t="n">
+        <v>44</v>
+      </c>
+      <c r="AO32" t="n">
+        <v>183</v>
+      </c>
+      <c r="AP32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR32" t="n">
+        <v>150</v>
+      </c>
+      <c r="AS32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV32" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW32" t="n">
+        <v>50</v>
+      </c>
+      <c r="AX32" t="n">
+        <v>60</v>
+      </c>
+      <c r="AY32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA32" t="n">
+        <v>3200000</v>
+      </c>
+      <c r="BB32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE32" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D33" t="n">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="E33" t="n">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="F33" t="n">
+        <v>53.11</v>
+      </c>
+      <c r="G33" t="n">
+        <v>53.11</v>
+      </c>
+      <c r="H33" t="n">
+        <v>72.56</v>
+      </c>
+      <c r="I33" t="n">
+        <v>90.80076435666172</v>
+      </c>
+      <c r="J33" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="K33" t="n">
+        <v>8719</v>
+      </c>
+      <c r="L33" t="n">
+        <v>8759</v>
+      </c>
+      <c r="M33" t="n">
+        <v>78.72</v>
+      </c>
+      <c r="N33" t="n">
+        <v>73.3</v>
+      </c>
+      <c r="O33" t="n">
+        <v>173.88</v>
+      </c>
+      <c r="P33" t="n">
+        <v>71.29000000000001</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>87590</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" t="n">
+        <v>1754.68</v>
+      </c>
+      <c r="T33" t="n">
+        <v>123200</v>
+      </c>
+      <c r="U33" t="n">
+        <v>201300</v>
+      </c>
+      <c r="V33" t="n">
+        <v>36744</v>
+      </c>
+      <c r="W33" t="n">
+        <v>27146</v>
+      </c>
+      <c r="X33" t="n">
+        <v>67653</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>167810</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN33" t="n">
+        <v>44</v>
+      </c>
+      <c r="AO33" t="n">
+        <v>183</v>
+      </c>
+      <c r="AP33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR33" t="n">
+        <v>150</v>
+      </c>
+      <c r="AS33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV33" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW33" t="n">
+        <v>50</v>
+      </c>
+      <c r="AX33" t="n">
+        <v>60</v>
+      </c>
+      <c r="AY33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA33" t="n">
+        <v>3200000</v>
+      </c>
+      <c r="BB33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE33" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" t="n">
+        <v>2024</v>
+      </c>
+      <c r="D34" t="n">
+        <v>79.11</v>
+      </c>
+      <c r="E34" t="n">
+        <v>79.11</v>
+      </c>
+      <c r="F34" t="n">
+        <v>71.54000000000001</v>
+      </c>
+      <c r="G34" t="n">
+        <v>71.54000000000001</v>
+      </c>
+      <c r="H34" t="n">
+        <v>75.48</v>
+      </c>
+      <c r="I34" t="n">
+        <v>87.26646435891597</v>
+      </c>
+      <c r="J34" t="n">
+        <v>100</v>
+      </c>
+      <c r="K34" t="n">
+        <v>8782</v>
+      </c>
+      <c r="L34" t="n">
+        <v>8782</v>
+      </c>
+      <c r="M34" t="n">
+        <v>72.68000000000001</v>
+      </c>
+      <c r="N34" t="n">
+        <v>64.28</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
+        <v>63.02</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>87820</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" t="n">
+        <v>1571.08</v>
+      </c>
+      <c r="T34" t="n">
+        <v>145200</v>
+      </c>
+      <c r="U34" t="n">
+        <v>219600</v>
+      </c>
+      <c r="V34" t="n">
+        <v>41442</v>
+      </c>
+      <c r="W34" t="n">
+        <v>27918</v>
+      </c>
+      <c r="X34" t="n">
+        <v>91709</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>183657</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN34" t="n">
+        <v>44</v>
+      </c>
+      <c r="AO34" t="n">
+        <v>183</v>
+      </c>
+      <c r="AP34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR34" t="n">
+        <v>150</v>
+      </c>
+      <c r="AS34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV34" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW34" t="n">
+        <v>50</v>
+      </c>
+      <c r="AX34" t="n">
+        <v>60</v>
+      </c>
+      <c r="AY34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA34" t="n">
+        <v>3200000</v>
+      </c>
+      <c r="BB34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE34" t="n">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>